<commit_message>
Update "Báo cáo OpenStack Queens"
</commit_message>
<xml_diff>
--- a/Queens/Install-manual/Linuxbridge/images/IP-Planning-Hardware-Requirements.xlsx
+++ b/Queens/Install-manual/Linuxbridge/images/IP-Planning-Hardware-Requirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNPT\thuctap012017\XuanSon\OpenStack\Install OpenStack\Pike\Install_OPS_with_Linuxbridge\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNPT\Install-OpenStack\Queens\Install-manual\Linuxbridge\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>Controller</t>
   </si>
@@ -101,12 +101,6 @@
     <t>10.10.10.72</t>
   </si>
   <si>
-    <t>OPS-setup</t>
-  </si>
-  <si>
-    <t>10.10.10.20</t>
-  </si>
-  <si>
     <t>192.168.2.71</t>
   </si>
   <si>
@@ -116,17 +110,17 @@
     <t>192.168.2.1</t>
   </si>
   <si>
-    <t>192.168.2.20</t>
-  </si>
-  <si>
     <t>IP PLANNING dành cho LAB OpenStack - Pike</t>
+  </si>
+  <si>
+    <t>IP PLANNING dành cho LAB OpenStack - Queens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,21 +155,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="0"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,12 +193,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -379,11 +354,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -502,27 +476,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -801,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:O24"/>
+  <dimension ref="C6:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="C16" sqref="C16:O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +774,7 @@
   <sheetData>
     <row r="6" spans="3:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="C6" s="29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -902,13 +857,13 @@
         <v>19</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>9</v>
@@ -956,13 +911,13 @@
         <v>19</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>9</v>
@@ -1005,7 +960,7 @@
     <row r="15" spans="3:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="3:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="C16" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
@@ -1081,99 +1036,99 @@
       </c>
     </row>
     <row r="19" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C19" s="40" t="s">
-        <v>23</v>
+      <c r="C19" s="32" t="s">
+        <v>0</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="17">
-        <v>1</v>
-      </c>
-      <c r="J19" s="17">
-        <v>1</v>
-      </c>
-      <c r="K19" s="42">
+      <c r="I19" s="37">
+        <v>6</v>
+      </c>
+      <c r="J19" s="38">
+        <v>2</v>
+      </c>
+      <c r="K19" s="39">
         <v>30</v>
       </c>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
     </row>
     <row r="20" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C20" s="41"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>2</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="18"/>
+      <c r="I20" s="22"/>
       <c r="J20" s="18"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
     </row>
     <row r="21" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C21" s="32" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="37">
-        <v>6</v>
-      </c>
-      <c r="J21" s="38">
-        <v>2</v>
-      </c>
-      <c r="K21" s="39">
+      <c r="I21" s="21">
+        <v>8</v>
+      </c>
+      <c r="J21" s="17">
+        <v>4</v>
+      </c>
+      <c r="K21" s="19">
         <v>30</v>
       </c>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
     </row>
     <row r="22" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C22" s="33"/>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>2</v>
@@ -1188,86 +1143,24 @@
       <c r="N22" s="35"/>
       <c r="O22" s="35"/>
     </row>
-    <row r="23" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C23" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="21">
-        <v>8</v>
-      </c>
-      <c r="J23" s="17">
-        <v>4</v>
-      </c>
-      <c r="K23" s="19">
-        <v>30</v>
-      </c>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-    </row>
-    <row r="24" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C24" s="33"/>
-      <c r="D24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
-    </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
+  <mergeCells count="38">
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
     <mergeCell ref="O19:O20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O23:O24"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="C6:O6"/>

</xml_diff>